<commit_message>
Mejora para obtener el df_fatiga_media
</commit_message>
<xml_diff>
--- a/Datos Sentadilla Frontal.xlsx
+++ b/Datos Sentadilla Frontal.xlsx
@@ -8,13 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="14">
   <si>
     <t>Ejercicio</t>
   </si>
@@ -53,6 +54,9 @@
   </si>
   <si>
     <t>C</t>
+  </si>
+  <si>
+    <t>Porcentaje de fatiga</t>
   </si>
 </sst>
 </file>
@@ -4448,4 +4452,135 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2">
+        <v>44956</v>
+      </c>
+      <c r="C2">
+        <v>13.28449328449329</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2">
+        <v>44964</v>
+      </c>
+      <c r="C3">
+        <v>12.57682177348552</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2">
+        <v>44966</v>
+      </c>
+      <c r="C4">
+        <v>20.94769321187188</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2">
+        <v>44971</v>
+      </c>
+      <c r="C5">
+        <v>17.34972677595628</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2">
+        <v>44976</v>
+      </c>
+      <c r="C6">
+        <v>6.451612903225811</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2">
+        <v>44978</v>
+      </c>
+      <c r="C7">
+        <v>18.64406779661016</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2">
+        <v>44980</v>
+      </c>
+      <c r="C8">
+        <v>18.57683982683983</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2">
+        <v>44984</v>
+      </c>
+      <c r="C9">
+        <v>14.3905360886493</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2">
+        <v>44986</v>
+      </c>
+      <c r="C10">
+        <v>16.12903225806451</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2">
+        <v>44991</v>
+      </c>
+      <c r="C11">
+        <v>21.66832834828847</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>